<commit_message>
#8 FIXME: tests does not yet fixed.
</commit_message>
<xml_diff>
--- a/test/読み取り元 src.xlsx
+++ b/test/読み取り元 src.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1e761a4b3430ee0/git_work/KubotaHA/TranscribeExcelData/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\hkubota\github\TranscribeExcelData\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{52B85099-6990-4320-9CD8-272625149E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF62DDCB-B609-4131-B26E-AE89907390A8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{675A58C6-99D5-4C3C-8D44-D52E4DF54CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35730" yWindow="4905" windowWidth="7695" windowHeight="23445" xr2:uid="{90AC207A-EF8E-49E0-BAC3-99B3184B1A4F}"/>
+    <workbookView xWindow="18840" yWindow="14910" windowWidth="25950" windowHeight="16095" xr2:uid="{90AC207A-EF8E-49E0-BAC3-99B3184B1A4F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="読み取り元" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -229,20 +229,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -561,9 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A32A39-1044-4546-9492-BA7EF3989C03}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -621,73 +613,31 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
@@ -698,7 +648,7 @@
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -706,7 +656,7 @@
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
     </row>
@@ -771,12 +721,12 @@
       </c>
     </row>
     <row r="44" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C44" s="4" t="s">
+      <c r="C44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.4">
-      <c r="C58" s="4" t="s">
+      <c r="C58" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>